<commit_message>
changes to all schema files and excel files
</commit_message>
<xml_diff>
--- a/Database Implementation/Test Data Generator - Adrian.xlsx
+++ b/Database Implementation/Test Data Generator - Adrian.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\501834813\Documents\GitHub\WebProject\Database Implementation\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="6000"/>
+    <workbookView windowWidth="19890" windowHeight="8520"/>
   </bookViews>
   <sheets>
     <sheet name="user_profile" sheetId="1" r:id="rId1"/>
@@ -17,12 +12,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">user_profile!$A$1:$L$52</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102">
   <si>
     <t>password_hash</t>
   </si>
@@ -66,30 +61,33 @@
     <t>john.doe@gmail.com</t>
   </si>
   <si>
+    <t>2000-01-01</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Gavin</t>
+  </si>
+  <si>
+    <t>Hunter</t>
+  </si>
+  <si>
+    <t>1990-01-01</t>
+  </si>
+  <si>
+    <t>Carol</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
     <t>Male</t>
   </si>
   <si>
-    <t>Female</t>
-  </si>
-  <si>
-    <t>Active</t>
-  </si>
-  <si>
-    <t>2000-01-01</t>
-  </si>
-  <si>
-    <t>Gavin</t>
-  </si>
-  <si>
-    <t>Hunter</t>
-  </si>
-  <si>
-    <t>Carol</t>
-  </si>
-  <si>
-    <t>James</t>
-  </si>
-  <si>
     <t>Yvonne</t>
   </si>
   <si>
@@ -322,9 +320,6 @@
   </si>
   <si>
     <t>Paige</t>
-  </si>
-  <si>
-    <t>1990-01-01</t>
   </si>
   <si>
     <t>https://homepage.net/name_generator/</t>
@@ -333,35 +328,55 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="20" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri Light"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -369,7 +384,31 @@
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -377,35 +416,58 @@
       <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <charset val="134"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -413,75 +475,22 @@
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C5700"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
   </fonts>
   <fills count="34">
@@ -493,180 +502,193 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -680,11 +702,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4"/>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -701,8 +729,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.39997558519241921"/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -718,6 +761,39 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.399975585192419"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -739,45 +815,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -786,134 +823,140 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10"/>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="43">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -962,7 +1005,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -995,26 +1038,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1047,23 +1073,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1205,40 +1214,35 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:L58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="162" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.2857142857143" customWidth="1"/>
+    <col min="2" max="2" width="12.4285714285714" customWidth="1"/>
+    <col min="3" max="3" width="11.5714285714286" customWidth="1"/>
+    <col min="4" max="4" width="20.2857142857143" customWidth="1"/>
+    <col min="5" max="5" width="15.8571428571429" customWidth="1"/>
+    <col min="6" max="6" width="5.42857142857143" customWidth="1"/>
+    <col min="7" max="7" width="21.2857142857143" customWidth="1"/>
+    <col min="8" max="8" width="20.1428571428571" customWidth="1"/>
+    <col min="9" max="9" width="22.8571428571429" customWidth="1"/>
+    <col min="10" max="10" width="20.1428571428571" customWidth="1"/>
+    <col min="11" max="11" width="13.4285714285714" customWidth="1"/>
+    <col min="12" max="12" width="162" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" ht="30.75" spans="1:12">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1277,18 +1281,18 @@
         <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('password_hash','first_name','sur_name','email','date_of_birth','sex','gender_preference','black_listed_user','black_listed_reason','user_status');</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" ht="30" spans="2:12">
       <c r="B2" t="s">
         <v>11</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>17</v>
+      <c r="E2" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -1302,24 +1306,24 @@
       <c r="K2" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="3" t="str">
+      <c r="L2" s="1" t="str">
         <f>"insert into user_profile ("&amp;$A$1&amp;","&amp;$B$1&amp;","&amp;$C$1&amp;","&amp;$D$1&amp;","&amp;$E$1&amp;","&amp;$F$1&amp;","&amp;$G$1&amp;","&amp;$H$1&amp;","&amp;$I$1&amp;","&amp;$K$1&amp;") values  ('"&amp;A2&amp;"','"&amp;B2&amp;"','"&amp;C2&amp;"','"&amp;D2&amp;"','"&amp;E2&amp;"','"&amp;F2&amp;"','"&amp;G2&amp;"','"&amp;H2&amp;"','"&amp;I2&amp;"','"&amp;K2&amp;"');"</f>
         <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','John','Doe','john.doe@gmail.com','2000-01-01','1','Female','0','','Active');</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" ht="30" spans="2:12">
       <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
         <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
       </c>
       <c r="D3" t="str">
         <f>B3&amp;"."&amp;C3&amp;"@gmail.com"</f>
         <v>Gavin.Hunter@gmail.com</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>100</v>
+      <c r="E3" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -1333,12 +1337,12 @@
       <c r="K3" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="3" t="str">
+      <c r="L3" s="1" t="str">
         <f t="shared" ref="L3:L52" si="0">"insert into user_profile ("&amp;$A$1&amp;","&amp;$B$1&amp;","&amp;$C$1&amp;","&amp;$D$1&amp;","&amp;$E$1&amp;","&amp;$F$1&amp;","&amp;$G$1&amp;","&amp;$H$1&amp;","&amp;$I$1&amp;","&amp;$K$1&amp;") values  ('"&amp;A3&amp;"','"&amp;B3&amp;"','"&amp;C3&amp;"','"&amp;D3&amp;"','"&amp;E3&amp;"','"&amp;F3&amp;"','"&amp;G3&amp;"','"&amp;H3&amp;"','"&amp;I3&amp;"','"&amp;K3&amp;"');"</f>
         <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Gavin','Hunter','Gavin.Hunter@gmail.com','1990-01-01','1','Female','0','','Active');</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" ht="30" spans="2:12">
       <c r="B4" t="s">
         <v>20</v>
       </c>
@@ -1349,14 +1353,14 @@
         <f t="shared" ref="D4:D52" si="1">B4&amp;"."&amp;C4&amp;"@gmail.com"</f>
         <v>Carol.James@gmail.com</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>100</v>
+      <c r="E4" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="F4">
         <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -1364,30 +1368,30 @@
       <c r="K4" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="3" t="str">
+      <c r="L4" s="1" t="str">
         <f t="shared" si="0"/>
         <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Carol','James','Carol.James@gmail.com','1990-01-01','2','Male','0','','Active');</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" ht="30" spans="2:12">
       <c r="B5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="1"/>
         <v>Yvonne.Edmunds@gmail.com</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>100</v>
+      <c r="E5" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="F5">
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -1395,24 +1399,24 @@
       <c r="K5" t="s">
         <v>16</v>
       </c>
-      <c r="L5" s="3" t="str">
+      <c r="L5" s="1" t="str">
         <f t="shared" si="0"/>
         <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Yvonne','Edmunds','Yvonne.Edmunds@gmail.com','1990-01-01','2','Male','0','','Active');</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" ht="30" spans="2:12">
       <c r="B6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="1"/>
         <v>Max.Glover@gmail.com</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>100</v>
+      <c r="E6" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -1426,24 +1430,24 @@
       <c r="K6" t="s">
         <v>16</v>
       </c>
-      <c r="L6" s="3" t="str">
+      <c r="L6" s="1" t="str">
         <f t="shared" si="0"/>
         <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Max','Glover','Max.Glover@gmail.com','1990-01-01','1','Female','0','','Active');</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" ht="30" spans="2:12">
       <c r="B7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="1"/>
         <v>Dan.King@gmail.com</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>100</v>
+      <c r="E7" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -1457,30 +1461,30 @@
       <c r="K7" t="s">
         <v>16</v>
       </c>
-      <c r="L7" s="3" t="str">
+      <c r="L7" s="1" t="str">
         <f t="shared" si="0"/>
         <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Dan','King','Dan.King@gmail.com','1990-01-01','1','Female','0','','Active');</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" ht="30" spans="2:12">
       <c r="B8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="1"/>
         <v>Carolyn.Thomson@gmail.com</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>100</v>
+      <c r="E8" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="F8">
         <v>2</v>
       </c>
       <c r="G8" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -1488,30 +1492,30 @@
       <c r="K8" t="s">
         <v>16</v>
       </c>
-      <c r="L8" s="3" t="str">
+      <c r="L8" s="1" t="str">
         <f t="shared" si="0"/>
         <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Carolyn','Thomson','Carolyn.Thomson@gmail.com','1990-01-01','2','Male','0','','Active');</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" ht="30" spans="2:12">
       <c r="B9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="1"/>
         <v>Angela.Martin@gmail.com</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>100</v>
+      <c r="E9" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="F9">
         <v>2</v>
       </c>
       <c r="G9" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -1519,30 +1523,30 @@
       <c r="K9" t="s">
         <v>16</v>
       </c>
-      <c r="L9" s="3" t="str">
+      <c r="L9" s="1" t="str">
         <f t="shared" si="0"/>
         <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Angela','Martin','Angela.Martin@gmail.com','1990-01-01','2','Male','0','','Active');</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" ht="30" spans="2:12">
       <c r="B10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="1"/>
         <v>Melanie.Slater@gmail.com</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>100</v>
+      <c r="E10" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="F10">
         <v>2</v>
       </c>
       <c r="G10" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -1550,30 +1554,30 @@
       <c r="K10" t="s">
         <v>16</v>
       </c>
-      <c r="L10" s="3" t="str">
+      <c r="L10" s="1" t="str">
         <f t="shared" si="0"/>
         <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Melanie','Slater','Melanie.Slater@gmail.com','1990-01-01','2','Male','0','','Active');</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" ht="30" spans="2:12">
       <c r="B11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="1"/>
         <v>Jennifer.Langdon@gmail.com</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>100</v>
+      <c r="E11" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="F11">
         <v>2</v>
       </c>
       <c r="G11" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -1581,24 +1585,24 @@
       <c r="K11" t="s">
         <v>16</v>
       </c>
-      <c r="L11" s="3" t="str">
+      <c r="L11" s="1" t="str">
         <f t="shared" si="0"/>
         <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Jennifer','Langdon','Jennifer.Langdon@gmail.com','1990-01-01','2','Male','0','','Active');</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" ht="30" spans="2:12">
       <c r="B12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="1"/>
         <v>Paul.Alsop@gmail.com</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>100</v>
+      <c r="E12" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -1612,24 +1616,24 @@
       <c r="K12" t="s">
         <v>16</v>
       </c>
-      <c r="L12" s="3" t="str">
+      <c r="L12" s="1" t="str">
         <f t="shared" si="0"/>
         <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Paul','Alsop','Paul.Alsop@gmail.com','1990-01-01','1','Female','0','','Active');</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" ht="30" spans="2:12">
       <c r="B13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="1"/>
         <v>Owen.Wilkins@gmail.com</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>100</v>
+      <c r="E13" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -1643,30 +1647,30 @@
       <c r="K13" t="s">
         <v>16</v>
       </c>
-      <c r="L13" s="3" t="str">
+      <c r="L13" s="1" t="str">
         <f t="shared" si="0"/>
         <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Owen','Wilkins','Owen.Wilkins@gmail.com','1990-01-01','1','Female','0','','Active');</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" ht="30" spans="2:12">
       <c r="B14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="1"/>
         <v>Ella.Taylor@gmail.com</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>100</v>
+      <c r="E14" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="F14">
         <v>2</v>
       </c>
       <c r="G14" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -1674,30 +1678,30 @@
       <c r="K14" t="s">
         <v>16</v>
       </c>
-      <c r="L14" s="3" t="str">
+      <c r="L14" s="1" t="str">
         <f t="shared" si="0"/>
         <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Ella','Taylor','Ella.Taylor@gmail.com','1990-01-01','2','Male','0','','Active');</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" ht="30" spans="2:12">
       <c r="B15" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="1"/>
         <v>Amanda.Young@gmail.com</v>
       </c>
-      <c r="E15" s="4" t="s">
-        <v>100</v>
+      <c r="E15" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="F15">
         <v>2</v>
       </c>
       <c r="G15" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -1705,30 +1709,30 @@
       <c r="K15" t="s">
         <v>16</v>
       </c>
-      <c r="L15" s="3" t="str">
+      <c r="L15" s="1" t="str">
         <f t="shared" si="0"/>
         <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Amanda','Young','Amanda.Young@gmail.com','1990-01-01','2','Male','0','','Active');</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" ht="30" spans="2:12">
       <c r="B16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="1"/>
         <v>Abigail.Mackay@gmail.com</v>
       </c>
-      <c r="E16" s="4" t="s">
-        <v>100</v>
+      <c r="E16" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="F16">
         <v>2</v>
       </c>
       <c r="G16" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H16">
         <v>0</v>
@@ -1736,30 +1740,30 @@
       <c r="K16" t="s">
         <v>16</v>
       </c>
-      <c r="L16" s="3" t="str">
+      <c r="L16" s="1" t="str">
         <f t="shared" si="0"/>
         <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Abigail','Mackay','Abigail.Mackay@gmail.com','1990-01-01','2','Male','0','','Active');</v>
       </c>
     </row>
-    <row r="17" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" ht="30" spans="2:12">
       <c r="B17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" si="1"/>
         <v>Lily.Avery@gmail.com</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>100</v>
+      <c r="E17" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="F17">
         <v>2</v>
       </c>
       <c r="G17" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -1767,30 +1771,30 @@
       <c r="K17" t="s">
         <v>16</v>
       </c>
-      <c r="L17" s="3" t="str">
+      <c r="L17" s="1" t="str">
         <f t="shared" si="0"/>
         <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Lily','Avery','Lily.Avery@gmail.com','1990-01-01','2','Male','0','','Active');</v>
       </c>
     </row>
-    <row r="18" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" ht="30" spans="2:12">
       <c r="B18" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C18" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="1"/>
         <v>Madeleine.Wilson@gmail.com</v>
       </c>
-      <c r="E18" s="4" t="s">
-        <v>100</v>
+      <c r="E18" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="F18">
         <v>2</v>
       </c>
       <c r="G18" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H18">
         <v>0</v>
@@ -1798,24 +1802,24 @@
       <c r="K18" t="s">
         <v>16</v>
       </c>
-      <c r="L18" s="3" t="str">
+      <c r="L18" s="1" t="str">
         <f t="shared" si="0"/>
         <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Madeleine','Wilson','Madeleine.Wilson@gmail.com','1990-01-01','2','Male','0','','Active');</v>
       </c>
     </row>
-    <row r="19" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" ht="30" spans="2:12">
       <c r="B19" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C19" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" si="1"/>
         <v>Carl.Stewart@gmail.com</v>
       </c>
-      <c r="E19" s="4" t="s">
-        <v>100</v>
+      <c r="E19" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -1829,14 +1833,14 @@
       <c r="K19" t="s">
         <v>16</v>
       </c>
-      <c r="L19" s="3" t="str">
+      <c r="L19" s="1" t="str">
         <f t="shared" si="0"/>
         <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Carl','Stewart','Carl.Stewart@gmail.com','1990-01-01','1','Female','0','','Active');</v>
       </c>
     </row>
-    <row r="20" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" ht="30" spans="2:12">
       <c r="B20" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C20" t="s">
         <v>21</v>
@@ -1845,14 +1849,14 @@
         <f t="shared" si="1"/>
         <v>Faith.James@gmail.com</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>100</v>
+      <c r="E20" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="F20">
         <v>2</v>
       </c>
       <c r="G20" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -1860,30 +1864,30 @@
       <c r="K20" t="s">
         <v>16</v>
       </c>
-      <c r="L20" s="3" t="str">
+      <c r="L20" s="1" t="str">
         <f t="shared" si="0"/>
         <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Faith','James','Faith.James@gmail.com','1990-01-01','2','Male','0','','Active');</v>
       </c>
     </row>
-    <row r="21" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" ht="30" spans="2:12">
       <c r="B21" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C21" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="1"/>
         <v>Lisa.Sharp@gmail.com</v>
       </c>
-      <c r="E21" s="4" t="s">
-        <v>100</v>
+      <c r="E21" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="F21">
         <v>2</v>
       </c>
       <c r="G21" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H21">
         <v>0</v>
@@ -1891,24 +1895,24 @@
       <c r="K21" t="s">
         <v>16</v>
       </c>
-      <c r="L21" s="3" t="str">
+      <c r="L21" s="1" t="str">
         <f t="shared" si="0"/>
         <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Lisa','Sharp','Lisa.Sharp@gmail.com','1990-01-01','2','Male','0','','Active');</v>
       </c>
     </row>
-    <row r="22" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" ht="30" spans="2:12">
       <c r="B22" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C22" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" si="1"/>
         <v>Lucas.Short@gmail.com</v>
       </c>
-      <c r="E22" s="4" t="s">
-        <v>100</v>
+      <c r="E22" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="F22">
         <v>1</v>
@@ -1922,30 +1926,30 @@
       <c r="K22" t="s">
         <v>16</v>
       </c>
-      <c r="L22" s="3" t="str">
+      <c r="L22" s="1" t="str">
         <f t="shared" si="0"/>
         <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Lucas','Short','Lucas.Short@gmail.com','1990-01-01','1','Female','0','','Active');</v>
       </c>
     </row>
-    <row r="23" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" ht="30" spans="2:12">
       <c r="B23" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C23" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" si="1"/>
         <v>Una.Nash@gmail.com</v>
       </c>
-      <c r="E23" s="4" t="s">
-        <v>100</v>
+      <c r="E23" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="F23">
         <v>2</v>
       </c>
       <c r="G23" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -1953,24 +1957,24 @@
       <c r="K23" t="s">
         <v>16</v>
       </c>
-      <c r="L23" s="3" t="str">
+      <c r="L23" s="1" t="str">
         <f t="shared" si="0"/>
         <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Una','Nash','Una.Nash@gmail.com','1990-01-01','2','Male','0','','Active');</v>
       </c>
     </row>
-    <row r="24" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" ht="30" spans="2:12">
       <c r="B24" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C24" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D24" t="str">
         <f t="shared" si="1"/>
         <v>Jacob.Newman@gmail.com</v>
       </c>
-      <c r="E24" s="4" t="s">
-        <v>100</v>
+      <c r="E24" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="F24">
         <v>1</v>
@@ -1984,30 +1988,30 @@
       <c r="K24" t="s">
         <v>16</v>
       </c>
-      <c r="L24" s="3" t="str">
+      <c r="L24" s="1" t="str">
         <f t="shared" si="0"/>
         <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Jacob','Newman','Jacob.Newman@gmail.com','1990-01-01','1','Female','0','','Active');</v>
       </c>
     </row>
-    <row r="25" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" ht="30" spans="2:12">
       <c r="B25" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C25" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D25" t="str">
         <f t="shared" si="1"/>
         <v>Dorothy.Mathis@gmail.com</v>
       </c>
-      <c r="E25" s="4" t="s">
-        <v>100</v>
+      <c r="E25" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="F25">
         <v>2</v>
       </c>
       <c r="G25" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H25">
         <v>0</v>
@@ -2015,30 +2019,30 @@
       <c r="K25" t="s">
         <v>16</v>
       </c>
-      <c r="L25" s="3" t="str">
+      <c r="L25" s="1" t="str">
         <f t="shared" si="0"/>
         <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Dorothy','Mathis','Dorothy.Mathis@gmail.com','1990-01-01','2','Male','0','','Active');</v>
       </c>
     </row>
-    <row r="26" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" ht="30" spans="2:12">
       <c r="B26" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C26" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D26" t="str">
         <f t="shared" si="1"/>
         <v>Irene.Hemmings@gmail.com</v>
       </c>
-      <c r="E26" s="4" t="s">
-        <v>100</v>
+      <c r="E26" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="F26">
         <v>2</v>
       </c>
       <c r="G26" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H26">
         <v>0</v>
@@ -2046,30 +2050,30 @@
       <c r="K26" t="s">
         <v>16</v>
       </c>
-      <c r="L26" s="3" t="str">
+      <c r="L26" s="1" t="str">
         <f t="shared" si="0"/>
         <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Irene','Hemmings','Irene.Hemmings@gmail.com','1990-01-01','2','Male','0','','Active');</v>
       </c>
     </row>
-    <row r="27" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" ht="30" spans="2:12">
       <c r="B27" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C27" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D27" t="str">
         <f t="shared" si="1"/>
         <v>Caroline.Davies@gmail.com</v>
       </c>
-      <c r="E27" s="4" t="s">
-        <v>100</v>
+      <c r="E27" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="F27">
         <v>2</v>
       </c>
       <c r="G27" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H27">
         <v>0</v>
@@ -2077,24 +2081,24 @@
       <c r="K27" t="s">
         <v>16</v>
       </c>
-      <c r="L27" s="3" t="str">
+      <c r="L27" s="1" t="str">
         <f t="shared" si="0"/>
         <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Caroline','Davies','Caroline.Davies@gmail.com','1990-01-01','2','Male','0','','Active');</v>
       </c>
     </row>
-    <row r="28" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" ht="30" spans="2:12">
       <c r="B28" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C28" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="1"/>
         <v>Phil.Sharp@gmail.com</v>
       </c>
-      <c r="E28" s="4" t="s">
-        <v>100</v>
+      <c r="E28" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="F28">
         <v>1</v>
@@ -2108,30 +2112,30 @@
       <c r="K28" t="s">
         <v>16</v>
       </c>
-      <c r="L28" s="3" t="str">
+      <c r="L28" s="1" t="str">
         <f t="shared" si="0"/>
         <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Phil','Sharp','Phil.Sharp@gmail.com','1990-01-01','1','Female','0','','Active');</v>
       </c>
     </row>
-    <row r="29" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" ht="30" spans="2:12">
       <c r="B29" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C29" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D29" t="str">
         <f t="shared" si="1"/>
         <v>Ella.Hughes@gmail.com</v>
       </c>
-      <c r="E29" s="4" t="s">
-        <v>100</v>
+      <c r="E29" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="F29">
         <v>2</v>
       </c>
       <c r="G29" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H29">
         <v>0</v>
@@ -2139,30 +2143,30 @@
       <c r="K29" t="s">
         <v>16</v>
       </c>
-      <c r="L29" s="3" t="str">
+      <c r="L29" s="1" t="str">
         <f t="shared" si="0"/>
         <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Ella','Hughes','Ella.Hughes@gmail.com','1990-01-01','2','Male','0','','Active');</v>
       </c>
     </row>
-    <row r="30" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" ht="30" spans="2:12">
       <c r="B30" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C30" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D30" t="str">
         <f t="shared" si="1"/>
         <v>Samantha.Ferguson@gmail.com</v>
       </c>
-      <c r="E30" s="4" t="s">
-        <v>100</v>
+      <c r="E30" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="F30">
         <v>2</v>
       </c>
       <c r="G30" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H30">
         <v>0</v>
@@ -2170,30 +2174,30 @@
       <c r="K30" t="s">
         <v>16</v>
       </c>
-      <c r="L30" s="3" t="str">
+      <c r="L30" s="1" t="str">
         <f t="shared" si="0"/>
         <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Samantha','Ferguson','Samantha.Ferguson@gmail.com','1990-01-01','2','Male','0','','Active');</v>
       </c>
     </row>
-    <row r="31" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" ht="30" spans="2:12">
       <c r="B31" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C31" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D31" t="str">
         <f t="shared" si="1"/>
         <v>Warren.Rutherford@gmail.com</v>
       </c>
-      <c r="E31" s="4" t="s">
-        <v>100</v>
+      <c r="E31" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="F31">
         <v>1</v>
       </c>
       <c r="G31" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H31">
         <v>0</v>
@@ -2201,247 +2205,247 @@
       <c r="K31" t="s">
         <v>16</v>
       </c>
-      <c r="L31" s="3" t="str">
+      <c r="L31" s="1" t="str">
         <f t="shared" si="0"/>
         <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Warren','Rutherford','Warren.Rutherford@gmail.com','1990-01-01','1','Male','0','','Active');</v>
       </c>
     </row>
-    <row r="32" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" ht="30" spans="2:12">
       <c r="B32" t="s">
+        <v>74</v>
+      </c>
+      <c r="C32" t="s">
+        <v>75</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="1"/>
+        <v>Elizabeth.Lewis@gmail.com</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F32">
+        <v>2</v>
+      </c>
+      <c r="G32" t="s">
+        <v>22</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="K32" t="s">
+        <v>16</v>
+      </c>
+      <c r="L32" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Elizabeth','Lewis','Elizabeth.Lewis@gmail.com','1990-01-01','2','Male','0','','Active');</v>
+      </c>
+    </row>
+    <row r="33" ht="30" spans="2:12">
+      <c r="B33" t="s">
+        <v>76</v>
+      </c>
+      <c r="C33" t="s">
+        <v>36</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="1"/>
+        <v>Jane.Langdon@gmail.com</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33">
+        <v>2</v>
+      </c>
+      <c r="G33" t="s">
+        <v>22</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="K33" t="s">
+        <v>16</v>
+      </c>
+      <c r="L33" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Jane','Langdon','Jane.Langdon@gmail.com','1990-01-01','2','Male','0','','Active');</v>
+      </c>
+    </row>
+    <row r="34" ht="30" spans="2:12">
+      <c r="B34" t="s">
+        <v>77</v>
+      </c>
+      <c r="C34" t="s">
+        <v>78</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="1"/>
+        <v>Ava.Pullman@gmail.com</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F34">
+        <v>2</v>
+      </c>
+      <c r="G34" t="s">
+        <v>22</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="K34" t="s">
+        <v>16</v>
+      </c>
+      <c r="L34" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Ava','Pullman','Ava.Pullman@gmail.com','1990-01-01','2','Male','0','','Active');</v>
+      </c>
+    </row>
+    <row r="35" ht="30" spans="2:12">
+      <c r="B35" t="s">
+        <v>79</v>
+      </c>
+      <c r="C35" t="s">
+        <v>80</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="1"/>
+        <v>Vanessa.Campbell@gmail.com</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F35">
+        <v>2</v>
+      </c>
+      <c r="G35" t="s">
+        <v>22</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="K35" t="s">
+        <v>16</v>
+      </c>
+      <c r="L35" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Vanessa','Campbell','Vanessa.Campbell@gmail.com','1990-01-01','2','Male','0','','Active');</v>
+      </c>
+    </row>
+    <row r="36" ht="30" spans="2:12">
+      <c r="B36" t="s">
+        <v>81</v>
+      </c>
+      <c r="C36" t="s">
+        <v>82</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="1"/>
+        <v>Diane.Henderson@gmail.com</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F36">
+        <v>2</v>
+      </c>
+      <c r="G36" t="s">
+        <v>22</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="K36" t="s">
+        <v>16</v>
+      </c>
+      <c r="L36" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Diane','Henderson','Diane.Henderson@gmail.com','1990-01-01','2','Male','0','','Active');</v>
+      </c>
+    </row>
+    <row r="37" ht="30" spans="2:12">
+      <c r="B37" t="s">
+        <v>49</v>
+      </c>
+      <c r="C37" t="s">
+        <v>83</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="1"/>
+        <v>Madeleine.Duncan@gmail.com</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F37">
+        <v>2</v>
+      </c>
+      <c r="G37" t="s">
+        <v>22</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="K37" t="s">
+        <v>16</v>
+      </c>
+      <c r="L37" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Madeleine','Duncan','Madeleine.Duncan@gmail.com','1990-01-01','2','Male','0','','Active');</v>
+      </c>
+    </row>
+    <row r="38" ht="30" spans="2:12">
+      <c r="B38" t="s">
+        <v>84</v>
+      </c>
+      <c r="C38" t="s">
+        <v>46</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="1"/>
+        <v>Diana.Mackay@gmail.com</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F38">
+        <v>2</v>
+      </c>
+      <c r="G38" t="s">
+        <v>22</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="K38" t="s">
+        <v>16</v>
+      </c>
+      <c r="L38" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Diana','Mackay','Diana.Mackay@gmail.com','1990-01-01','2','Male','0','','Active');</v>
+      </c>
+    </row>
+    <row r="39" ht="30" spans="2:12">
+      <c r="B39" t="s">
+        <v>58</v>
+      </c>
+      <c r="C39" t="s">
         <v>73</v>
       </c>
-      <c r="C32" t="s">
-        <v>74</v>
-      </c>
-      <c r="D32" t="str">
-        <f t="shared" si="1"/>
-        <v>Elizabeth.Lewis@gmail.com</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="F32">
-        <v>2</v>
-      </c>
-      <c r="G32" t="s">
-        <v>14</v>
-      </c>
-      <c r="H32">
-        <v>0</v>
-      </c>
-      <c r="K32" t="s">
-        <v>16</v>
-      </c>
-      <c r="L32" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Elizabeth','Lewis','Elizabeth.Lewis@gmail.com','1990-01-01','2','Male','0','','Active');</v>
-      </c>
-    </row>
-    <row r="33" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>75</v>
-      </c>
-      <c r="C33" t="s">
-        <v>35</v>
-      </c>
-      <c r="D33" t="str">
-        <f t="shared" si="1"/>
-        <v>Jane.Langdon@gmail.com</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="F33">
-        <v>2</v>
-      </c>
-      <c r="G33" t="s">
-        <v>14</v>
-      </c>
-      <c r="H33">
-        <v>0</v>
-      </c>
-      <c r="K33" t="s">
-        <v>16</v>
-      </c>
-      <c r="L33" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Jane','Langdon','Jane.Langdon@gmail.com','1990-01-01','2','Male','0','','Active');</v>
-      </c>
-    </row>
-    <row r="34" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>76</v>
-      </c>
-      <c r="C34" t="s">
-        <v>77</v>
-      </c>
-      <c r="D34" t="str">
-        <f t="shared" si="1"/>
-        <v>Ava.Pullman@gmail.com</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="F34">
-        <v>2</v>
-      </c>
-      <c r="G34" t="s">
-        <v>14</v>
-      </c>
-      <c r="H34">
-        <v>0</v>
-      </c>
-      <c r="K34" t="s">
-        <v>16</v>
-      </c>
-      <c r="L34" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Ava','Pullman','Ava.Pullman@gmail.com','1990-01-01','2','Male','0','','Active');</v>
-      </c>
-    </row>
-    <row r="35" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>78</v>
-      </c>
-      <c r="C35" t="s">
-        <v>79</v>
-      </c>
-      <c r="D35" t="str">
-        <f t="shared" si="1"/>
-        <v>Vanessa.Campbell@gmail.com</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="F35">
-        <v>2</v>
-      </c>
-      <c r="G35" t="s">
-        <v>14</v>
-      </c>
-      <c r="H35">
-        <v>0</v>
-      </c>
-      <c r="K35" t="s">
-        <v>16</v>
-      </c>
-      <c r="L35" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Vanessa','Campbell','Vanessa.Campbell@gmail.com','1990-01-01','2','Male','0','','Active');</v>
-      </c>
-    </row>
-    <row r="36" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>80</v>
-      </c>
-      <c r="C36" t="s">
-        <v>81</v>
-      </c>
-      <c r="D36" t="str">
-        <f t="shared" si="1"/>
-        <v>Diane.Henderson@gmail.com</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="F36">
-        <v>2</v>
-      </c>
-      <c r="G36" t="s">
-        <v>14</v>
-      </c>
-      <c r="H36">
-        <v>0</v>
-      </c>
-      <c r="K36" t="s">
-        <v>16</v>
-      </c>
-      <c r="L36" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Diane','Henderson','Diane.Henderson@gmail.com','1990-01-01','2','Male','0','','Active');</v>
-      </c>
-    </row>
-    <row r="37" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>48</v>
-      </c>
-      <c r="C37" t="s">
-        <v>82</v>
-      </c>
-      <c r="D37" t="str">
-        <f t="shared" si="1"/>
-        <v>Madeleine.Duncan@gmail.com</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="F37">
-        <v>2</v>
-      </c>
-      <c r="G37" t="s">
-        <v>14</v>
-      </c>
-      <c r="H37">
-        <v>0</v>
-      </c>
-      <c r="K37" t="s">
-        <v>16</v>
-      </c>
-      <c r="L37" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Madeleine','Duncan','Madeleine.Duncan@gmail.com','1990-01-01','2','Male','0','','Active');</v>
-      </c>
-    </row>
-    <row r="38" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>83</v>
-      </c>
-      <c r="C38" t="s">
-        <v>45</v>
-      </c>
-      <c r="D38" t="str">
-        <f t="shared" si="1"/>
-        <v>Diana.Mackay@gmail.com</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="F38">
-        <v>2</v>
-      </c>
-      <c r="G38" t="s">
-        <v>14</v>
-      </c>
-      <c r="H38">
-        <v>0</v>
-      </c>
-      <c r="K38" t="s">
-        <v>16</v>
-      </c>
-      <c r="L38" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Diana','Mackay','Diana.Mackay@gmail.com','1990-01-01','2','Male','0','','Active');</v>
-      </c>
-    </row>
-    <row r="39" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>57</v>
-      </c>
-      <c r="C39" t="s">
-        <v>72</v>
-      </c>
       <c r="D39" t="str">
         <f t="shared" si="1"/>
         <v>Una.Rutherford@gmail.com</v>
       </c>
-      <c r="E39" s="4" t="s">
-        <v>100</v>
+      <c r="E39" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="F39">
         <v>2</v>
       </c>
       <c r="G39" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H39">
         <v>0</v>
@@ -2449,24 +2453,24 @@
       <c r="K39" t="s">
         <v>16</v>
       </c>
-      <c r="L39" s="3" t="str">
+      <c r="L39" s="1" t="str">
         <f t="shared" si="0"/>
         <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Una','Rutherford','Una.Rutherford@gmail.com','1990-01-01','2','Male','0','','Active');</v>
       </c>
     </row>
-    <row r="40" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" ht="30" spans="2:12">
       <c r="B40" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C40" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D40" t="str">
         <f t="shared" si="1"/>
         <v>Jessica.Walsh@gmail.com</v>
       </c>
-      <c r="E40" s="4" t="s">
-        <v>100</v>
+      <c r="E40" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="F40">
         <v>2</v>
@@ -2480,24 +2484,24 @@
       <c r="K40" t="s">
         <v>16</v>
       </c>
-      <c r="L40" s="3" t="str">
+      <c r="L40" s="1" t="str">
         <f t="shared" si="0"/>
         <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Jessica','Walsh','Jessica.Walsh@gmail.com','1990-01-01','2','Female','0','','Active');</v>
       </c>
     </row>
-    <row r="41" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" ht="30" spans="2:12">
       <c r="B41" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C41" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D41" t="str">
         <f t="shared" si="1"/>
         <v>Ella.Terry@gmail.com</v>
       </c>
-      <c r="E41" s="4" t="s">
-        <v>100</v>
+      <c r="E41" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="F41">
         <v>2</v>
@@ -2511,30 +2515,30 @@
       <c r="K41" t="s">
         <v>16</v>
       </c>
-      <c r="L41" s="3" t="str">
+      <c r="L41" s="1" t="str">
         <f t="shared" si="0"/>
         <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Ella','Terry','Ella.Terry@gmail.com','1990-01-01','2','Female','0','','Active');</v>
       </c>
     </row>
-    <row r="42" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" ht="30" spans="2:12">
       <c r="B42" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C42" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D42" t="str">
         <f t="shared" si="1"/>
         <v>Robert.Wilkins@gmail.com</v>
       </c>
-      <c r="E42" s="4" t="s">
-        <v>100</v>
+      <c r="E42" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="F42">
         <v>1</v>
       </c>
       <c r="G42" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H42">
         <v>0</v>
@@ -2542,24 +2546,24 @@
       <c r="K42" t="s">
         <v>16</v>
       </c>
-      <c r="L42" s="3" t="str">
+      <c r="L42" s="1" t="str">
         <f t="shared" si="0"/>
         <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Robert','Wilkins','Robert.Wilkins@gmail.com','1990-01-01','1','Male','0','','Active');</v>
       </c>
     </row>
-    <row r="43" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" ht="30" spans="2:12">
       <c r="B43" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C43" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D43" t="str">
         <f t="shared" si="1"/>
         <v>Bella.Walsh@gmail.com</v>
       </c>
-      <c r="E43" s="4" t="s">
-        <v>100</v>
+      <c r="E43" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="F43">
         <v>2</v>
@@ -2573,24 +2577,24 @@
       <c r="K43" t="s">
         <v>16</v>
       </c>
-      <c r="L43" s="3" t="str">
+      <c r="L43" s="1" t="str">
         <f t="shared" si="0"/>
         <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Bella','Walsh','Bella.Walsh@gmail.com','1990-01-01','2','Female','0','','Active');</v>
       </c>
     </row>
-    <row r="44" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" ht="30" spans="2:12">
       <c r="B44" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C44" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D44" t="str">
         <f t="shared" si="1"/>
         <v>Penelope.Mackay@gmail.com</v>
       </c>
-      <c r="E44" s="4" t="s">
-        <v>100</v>
+      <c r="E44" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="F44">
         <v>2</v>
@@ -2604,24 +2608,24 @@
       <c r="K44" t="s">
         <v>16</v>
       </c>
-      <c r="L44" s="3" t="str">
+      <c r="L44" s="1" t="str">
         <f t="shared" si="0"/>
         <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Penelope','Mackay','Penelope.Mackay@gmail.com','1990-01-01','2','Female','0','','Active');</v>
       </c>
     </row>
-    <row r="45" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" ht="30" spans="2:12">
       <c r="B45" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C45" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D45" t="str">
         <f t="shared" si="1"/>
         <v>Amanda.Hart@gmail.com</v>
       </c>
-      <c r="E45" s="4" t="s">
-        <v>100</v>
+      <c r="E45" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="F45">
         <v>2</v>
@@ -2635,24 +2639,24 @@
       <c r="K45" t="s">
         <v>16</v>
       </c>
-      <c r="L45" s="3" t="str">
+      <c r="L45" s="1" t="str">
         <f t="shared" si="0"/>
         <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Amanda','Hart','Amanda.Hart@gmail.com','1990-01-01','2','Female','0','','Active');</v>
       </c>
     </row>
-    <row r="46" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" ht="30" spans="2:12">
       <c r="B46" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C46" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D46" t="str">
         <f t="shared" si="1"/>
         <v>Virginia.Randall@gmail.com</v>
       </c>
-      <c r="E46" s="4" t="s">
-        <v>100</v>
+      <c r="E46" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="F46">
         <v>2</v>
@@ -2666,24 +2670,24 @@
       <c r="K46" t="s">
         <v>16</v>
       </c>
-      <c r="L46" s="3" t="str">
+      <c r="L46" s="1" t="str">
         <f t="shared" si="0"/>
         <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Virginia','Randall','Virginia.Randall@gmail.com','1990-01-01','2','Female','0','','Active');</v>
       </c>
     </row>
-    <row r="47" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" ht="30" spans="2:12">
       <c r="B47" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C47" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D47" t="str">
         <f t="shared" si="1"/>
         <v>Gabrielle.Edmunds@gmail.com</v>
       </c>
-      <c r="E47" s="4" t="s">
-        <v>100</v>
+      <c r="E47" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="F47">
         <v>2</v>
@@ -2697,24 +2701,24 @@
       <c r="K47" t="s">
         <v>16</v>
       </c>
-      <c r="L47" s="3" t="str">
+      <c r="L47" s="1" t="str">
         <f t="shared" si="0"/>
         <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Gabrielle','Edmunds','Gabrielle.Edmunds@gmail.com','1990-01-01','2','Female','0','','Active');</v>
       </c>
     </row>
-    <row r="48" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" ht="30" spans="2:12">
       <c r="B48" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C48" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D48" t="str">
         <f t="shared" si="1"/>
         <v>Jessica.Anderson@gmail.com</v>
       </c>
-      <c r="E48" s="4" t="s">
-        <v>100</v>
+      <c r="E48" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="F48">
         <v>2</v>
@@ -2728,30 +2732,30 @@
       <c r="K48" t="s">
         <v>16</v>
       </c>
-      <c r="L48" s="3" t="str">
+      <c r="L48" s="1" t="str">
         <f t="shared" si="0"/>
         <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Jessica','Anderson','Jessica.Anderson@gmail.com','1990-01-01','2','Female','0','','Active');</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" ht="30" spans="2:12">
       <c r="B49" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C49" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D49" t="str">
         <f t="shared" si="1"/>
         <v>Jan.Buckland@gmail.com</v>
       </c>
-      <c r="E49" s="4" t="s">
-        <v>100</v>
+      <c r="E49" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="F49">
         <v>1</v>
       </c>
       <c r="G49" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H49">
         <v>0</v>
@@ -2759,14 +2763,14 @@
       <c r="K49" t="s">
         <v>16</v>
       </c>
-      <c r="L49" s="3" t="str">
+      <c r="L49" s="1" t="str">
         <f t="shared" si="0"/>
         <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Jan','Buckland','Jan.Buckland@gmail.com','1990-01-01','1','Male','0','','Active');</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" ht="30" spans="2:12">
       <c r="B50" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C50" t="s">
         <v>21</v>
@@ -2775,14 +2779,14 @@
         <f t="shared" si="1"/>
         <v>Stewart.James@gmail.com</v>
       </c>
-      <c r="E50" s="4" t="s">
-        <v>100</v>
+      <c r="E50" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="F50">
         <v>1</v>
       </c>
       <c r="G50" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H50">
         <v>0</v>
@@ -2790,24 +2794,24 @@
       <c r="K50" t="s">
         <v>16</v>
       </c>
-      <c r="L50" s="3" t="str">
+      <c r="L50" s="1" t="str">
         <f t="shared" si="0"/>
         <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Stewart','James','Stewart.James@gmail.com','1990-01-01','1','Male','0','','Active');</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" ht="30" spans="2:12">
       <c r="B51" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C51" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D51" t="str">
         <f t="shared" si="1"/>
         <v>Emma.White@gmail.com</v>
       </c>
-      <c r="E51" s="4" t="s">
-        <v>100</v>
+      <c r="E51" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="F51">
         <v>2</v>
@@ -2821,24 +2825,24 @@
       <c r="K51" t="s">
         <v>16</v>
       </c>
-      <c r="L51" s="3" t="str">
+      <c r="L51" s="1" t="str">
         <f t="shared" si="0"/>
         <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Emma','White','Emma.White@gmail.com','1990-01-01','2','Female','0','','Active');</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" ht="30" spans="2:12">
       <c r="B52" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C52" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D52" t="str">
         <f t="shared" si="1"/>
         <v>Lily.Paige@gmail.com</v>
       </c>
-      <c r="E52" s="4" t="s">
-        <v>100</v>
+      <c r="E52" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="F52">
         <v>2</v>
@@ -2852,22 +2856,25 @@
       <c r="K52" t="s">
         <v>16</v>
       </c>
-      <c r="L52" s="3" t="str">
+      <c r="L52" s="1" t="str">
         <f t="shared" si="0"/>
         <v>insert into user_profile (password_hash,first_name,sur_name,email,date_of_birth,sex,gender_preference,black_listed_user,black_listed_reason,user_status) values  ('','Lily','Paige','Lily.Paige@gmail.com','1990-01-01','2','Female','0','','Active');</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1">
       <c r="A58" t="s">
         <v>101</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L52"/>
+  <autoFilter ref="A1:L52">
+    <extLst/>
+  </autoFilter>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId1" display="john.doe@gmail.com"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>